<commit_message>
Graficos de distribuciones y las medias
</commit_message>
<xml_diff>
--- a/Datos_experto.xlsx
+++ b/Datos_experto.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\GitHub\Trabajo-Final-Bayesiana\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57300\Documents\GitHub\Trabajo-Final-Bayesiana\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{369BB945-A4F5-4303-AB5C-B95E4EDAAB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EC784D0B-9C9E-4044-BB2E-3D86CCD689DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -32,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -98,7 +108,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -110,7 +120,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -157,6 +167,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -192,6 +219,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -343,16 +387,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43234CD3-795E-45D9-A462-7170894B0B77}">
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection sqref="A1:C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -363,7 +407,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -374,7 +418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5</v>
       </c>
@@ -385,7 +429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>10</v>
       </c>
@@ -396,7 +440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>15</v>
       </c>
@@ -407,7 +451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>20</v>
       </c>
@@ -418,7 +462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>25</v>
       </c>
@@ -429,62 +473,62 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>30</v>
       </c>
       <c r="B8">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C8">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>35</v>
       </c>
       <c r="B9">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C9">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>40</v>
       </c>
       <c r="B10">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C10">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>45</v>
       </c>
       <c r="B11">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C11">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>50</v>
       </c>
       <c r="B12">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C12">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>55</v>
       </c>
@@ -495,7 +539,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>60</v>
       </c>
@@ -506,7 +550,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>65</v>
       </c>
@@ -517,7 +561,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>70</v>
       </c>
@@ -528,7 +572,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>75</v>
       </c>
@@ -539,7 +583,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>80</v>
       </c>
@@ -550,7 +594,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>85</v>
       </c>
@@ -561,7 +605,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>90</v>
       </c>
@@ -572,7 +616,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>95</v>
       </c>
@@ -583,7 +627,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>100</v>
       </c>
@@ -594,7 +638,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>105</v>
       </c>
@@ -605,7 +649,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>110</v>
       </c>
@@ -616,7 +660,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>115</v>
       </c>
@@ -627,7 +671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>120</v>
       </c>
@@ -638,7 +682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>125</v>
       </c>
@@ -649,7 +693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>130</v>
       </c>
@@ -660,7 +704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>135</v>
       </c>
@@ -671,7 +715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>140</v>
       </c>
@@ -682,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>145</v>
       </c>
@@ -693,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
simulación para obtener la distribución apriori
</commit_message>
<xml_diff>
--- a/Datos_experto.xlsx
+++ b/Datos_experto.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57300\Documents\GitHub\Trabajo-Final-Bayesiana\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\GitHub\Trabajo-Final-Bayesiana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{369BB945-A4F5-4303-AB5C-B95E4EDAAB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EC784D0B-9C9E-4044-BB2E-3D86CCD689DA}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,15 +33,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Precio</t>
+  </si>
+  <si>
+    <t>modelo_2012</t>
+  </si>
+  <si>
+    <t>modelo_2016</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -72,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,27 +393,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43234CD3-795E-45D9-A462-7170894B0B77}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C32"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>2012</v>
-      </c>
-      <c r="C1">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -418,7 +424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -429,7 +435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -440,7 +446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -451,7 +457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -462,7 +468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -473,7 +479,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -484,7 +490,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>35</v>
       </c>
@@ -495,7 +501,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -506,7 +512,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>45</v>
       </c>
@@ -517,7 +523,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50</v>
       </c>
@@ -528,7 +534,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>55</v>
       </c>
@@ -539,7 +545,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>60</v>
       </c>
@@ -550,7 +556,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>65</v>
       </c>
@@ -561,7 +567,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>70</v>
       </c>
@@ -572,7 +578,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>75</v>
       </c>
@@ -583,7 +589,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>80</v>
       </c>
@@ -594,7 +600,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>85</v>
       </c>
@@ -605,7 +611,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>90</v>
       </c>
@@ -616,7 +622,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>95</v>
       </c>
@@ -627,7 +633,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>100</v>
       </c>
@@ -638,7 +644,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>105</v>
       </c>
@@ -649,7 +655,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>110</v>
       </c>
@@ -660,7 +666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>115</v>
       </c>
@@ -671,7 +677,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>120</v>
       </c>
@@ -682,7 +688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>125</v>
       </c>
@@ -693,7 +699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>130</v>
       </c>
@@ -704,7 +710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>135</v>
       </c>
@@ -715,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>140</v>
       </c>
@@ -726,7 +732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>145</v>
       </c>
@@ -737,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Inclusion de la muestra
</commit_message>
<xml_diff>
--- a/Datos_experto.xlsx
+++ b/Datos_experto.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +429,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -440,10 +440,10 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -454,7 +454,7 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -465,7 +465,7 @@
         <v>20</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -473,10 +473,10 @@
         <v>25</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -484,7 +484,7 @@
         <v>30</v>
       </c>
       <c r="B8">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -495,10 +495,10 @@
         <v>35</v>
       </c>
       <c r="B9">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -506,10 +506,10 @@
         <v>40</v>
       </c>
       <c r="B10">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="C10">
-        <v>35</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -517,10 +517,10 @@
         <v>45</v>
       </c>
       <c r="B11">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -528,10 +528,10 @@
         <v>50</v>
       </c>
       <c r="B12">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>60</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -539,7 +539,7 @@
         <v>55</v>
       </c>
       <c r="B13">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>90</v>
@@ -550,10 +550,10 @@
         <v>60</v>
       </c>
       <c r="B14">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>95</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -561,10 +561,10 @@
         <v>65</v>
       </c>
       <c r="B15">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>90</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -572,10 +572,10 @@
         <v>70</v>
       </c>
       <c r="B16">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -583,10 +583,10 @@
         <v>75</v>
       </c>
       <c r="B17">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -594,10 +594,10 @@
         <v>80</v>
       </c>
       <c r="B18">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -605,10 +605,10 @@
         <v>85</v>
       </c>
       <c r="B19">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -616,10 +616,10 @@
         <v>90</v>
       </c>
       <c r="B20">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -627,10 +627,10 @@
         <v>95</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -638,10 +638,10 @@
         <v>100</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -649,10 +649,10 @@
         <v>105</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -663,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -674,7 +674,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -696,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>